<commit_message>
đang làm upload giảng viên
</commit_message>
<xml_diff>
--- a/public/uploadsgiangvien.xlsx
+++ b/public/uploadsgiangvien.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>giảng viên 1</t>
   </si>
@@ -28,6 +28,117 @@
   </si>
   <si>
     <t>gv4</t>
+  </si>
+  <si>
+    <t>gv1</t>
+  </si>
+  <si>
+    <t>gv2</t>
+  </si>
+  <si>
+    <t>gv3</t>
+  </si>
+  <si>
+    <t>giảng viên 2</t>
+  </si>
+  <si>
+    <t>gv2@gmail.com</t>
+  </si>
+  <si>
+    <t>giảng viên 3</t>
+  </si>
+  <si>
+    <t>giảng viên 4</t>
+  </si>
+  <si>
+    <t>gv5</t>
+  </si>
+  <si>
+    <t>giảng viên 5</t>
+  </si>
+  <si>
+    <t>gv6</t>
+  </si>
+  <si>
+    <t>giảng viên 6</t>
+  </si>
+  <si>
+    <t>gv7</t>
+  </si>
+  <si>
+    <t>giảng viên 7</t>
+  </si>
+  <si>
+    <t>gv8</t>
+  </si>
+  <si>
+    <t>giảng viên 8</t>
+  </si>
+  <si>
+    <t>gv9</t>
+  </si>
+  <si>
+    <t>giảng viên 9</t>
+  </si>
+  <si>
+    <t>gv10</t>
+  </si>
+  <si>
+    <t>giảng viên 10</t>
+  </si>
+  <si>
+    <t>gv11</t>
+  </si>
+  <si>
+    <t>giảng viên 11</t>
+  </si>
+  <si>
+    <t>gv12</t>
+  </si>
+  <si>
+    <t>giảng viên 12</t>
+  </si>
+  <si>
+    <t>gv13</t>
+  </si>
+  <si>
+    <t>giảng viên 13</t>
+  </si>
+  <si>
+    <t>gv14</t>
+  </si>
+  <si>
+    <t>giảng viên 14</t>
+  </si>
+  <si>
+    <t>gv15</t>
+  </si>
+  <si>
+    <t>giảng viên 15</t>
+  </si>
+  <si>
+    <t>gv16</t>
+  </si>
+  <si>
+    <t>giảng viên 16</t>
+  </si>
+  <si>
+    <t>gv17</t>
+  </si>
+  <si>
+    <t>giảng viên 17</t>
+  </si>
+  <si>
+    <t>gv18</t>
+  </si>
+  <si>
+    <t>giảng viên 18</t>
+  </si>
+  <si>
+    <t>gv19</t>
+  </si>
+  <si>
+    <t>giảng viên 19</t>
   </si>
 </sst>
 </file>
@@ -377,15 +488,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -398,14 +511,278 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="C11" r:id="rId7"/>
+    <hyperlink ref="C13" r:id="rId8"/>
+    <hyperlink ref="C15" r:id="rId9"/>
+    <hyperlink ref="C17" r:id="rId10"/>
+    <hyperlink ref="C19" r:id="rId11" display="gv2@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId12"/>
+    <hyperlink ref="C6" r:id="rId13"/>
+    <hyperlink ref="C8" r:id="rId14"/>
+    <hyperlink ref="C10" r:id="rId15"/>
+    <hyperlink ref="C12" r:id="rId16"/>
+    <hyperlink ref="C14" r:id="rId17"/>
+    <hyperlink ref="C16" r:id="rId18"/>
+    <hyperlink ref="C18" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hủy bỏ đăng nhập sau khi đóng trình duyệt
</commit_message>
<xml_diff>
--- a/public/uploadsgiangvien.xlsx
+++ b/public/uploadsgiangvien.xlsx
@@ -27,18 +27,6 @@
     <t>cntt</t>
   </si>
   <si>
-    <t>gv4</t>
-  </si>
-  <si>
-    <t>gv1</t>
-  </si>
-  <si>
-    <t>gv2</t>
-  </si>
-  <si>
-    <t>gv3</t>
-  </si>
-  <si>
     <t>giảng viên 2</t>
   </si>
   <si>
@@ -51,33 +39,18 @@
     <t>giảng viên 4</t>
   </si>
   <si>
-    <t>gv5</t>
-  </si>
-  <si>
     <t>giảng viên 5</t>
   </si>
   <si>
-    <t>gv6</t>
-  </si>
-  <si>
     <t>giảng viên 6</t>
   </si>
   <si>
-    <t>gv7</t>
-  </si>
-  <si>
     <t>giảng viên 7</t>
   </si>
   <si>
-    <t>gv8</t>
-  </si>
-  <si>
     <t>giảng viên 8</t>
   </si>
   <si>
-    <t>gv9</t>
-  </si>
-  <si>
     <t>giảng viên 9</t>
   </si>
   <si>
@@ -139,6 +112,33 @@
   </si>
   <si>
     <t>giảng viên 19</t>
+  </si>
+  <si>
+    <t>gv01</t>
+  </si>
+  <si>
+    <t>gv02</t>
+  </si>
+  <si>
+    <t>gv03</t>
+  </si>
+  <si>
+    <t>gv04</t>
+  </si>
+  <si>
+    <t>gv05</t>
+  </si>
+  <si>
+    <t>gv06</t>
+  </si>
+  <si>
+    <t>gv07</t>
+  </si>
+  <si>
+    <t>gv08</t>
+  </si>
+  <si>
+    <t>gv09</t>
   </si>
 </sst>
 </file>
@@ -490,15 +490,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -512,13 +512,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -526,10 +526,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -540,13 +540,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -554,10 +554,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -568,13 +568,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
@@ -582,10 +582,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
@@ -596,13 +596,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>2</v>
@@ -610,10 +610,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
@@ -624,13 +624,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -638,10 +638,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
@@ -652,13 +652,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
@@ -666,10 +666,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1</v>
@@ -680,13 +680,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
@@ -708,13 +708,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
@@ -722,10 +722,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
@@ -736,13 +736,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>2</v>
@@ -750,10 +750,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1</v>

</xml_diff>